<commit_message>
June 2020 regenerated sched
</commit_message>
<xml_diff>
--- a/HolidayShift.xlsx
+++ b/HolidayShift.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meryll\Dyna\monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8606EB0-AB07-4FC8-8953-DC5A84F0429F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B7942-BB82-4A00-A68C-D3B5C77BDD5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="3408" windowWidth="17280" windowHeight="9288" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1920" windowWidth="23040" windowHeight="6204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2062,10 +2062,10 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
         <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2096,10 +2096,10 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2130,10 +2130,10 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2150,7 +2150,7 @@
         <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
upload changes in output files
</commit_message>
<xml_diff>
--- a/HolidayShift.xlsx
+++ b/HolidayShift.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12345" activeTab="5"/>
+    <workbookView windowWidth="27945" windowHeight="12180" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -14,13 +13,28 @@
     <sheet name="2021" sheetId="4" r:id="rId4"/>
     <sheet name="2022" sheetId="5" r:id="rId5"/>
     <sheet name="2023" sheetId="6" r:id="rId6"/>
+    <sheet name="2024" sheetId="7" r:id="rId7"/>
+    <sheet name="2025" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="217">
   <si>
     <t>ts</t>
   </si>
@@ -620,20 +634,71 @@
   </si>
   <si>
     <t>Leb</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Rog</t>
+  </si>
+  <si>
+    <t>Cesca</t>
+  </si>
+  <si>
+    <t>Les</t>
+  </si>
+  <si>
+    <t>Chlo</t>
+  </si>
+  <si>
+    <t>Lance</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Elyse</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Lei</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Bon</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>Aime</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>ComRAR</t>
+  </si>
+  <si>
+    <t>CV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;₱&quot;* #,##0_-;\-&quot;₱&quot;* #,##0_-;_-&quot;₱&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;₱&quot;* #,##0_-;\-&quot;₱&quot;* #,##0_-;_-&quot;₱&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,38 +721,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="6"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3" tint="0.4"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="4"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -701,11 +764,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -732,18 +818,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -755,31 +834,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -794,7 +858,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -809,7 +901,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,19 +1009,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,103 +1039,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -959,25 +1051,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1019,6 +1111,54 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1051,54 +1191,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1118,10 +1210,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1130,140 +1225,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1271,55 +1363,63 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1330,6 +1430,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1620,10 +1727,13 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="4.14285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -5314,15 +5424,1055 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>44927.3125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>44927.8125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>44928.3125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>44928.8125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>44981.8125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>44962.3125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>44968.3125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
+        <v>44969.3125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
+        <v>44982.3125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
+        <v>44982.8125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2">
+        <v>45021.8125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2">
+        <v>45022.3125</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2">
+        <v>45022.8125</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
+        <v>45023.3125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
+        <v>45023.8125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
+        <v>45024.3125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
+        <v>45024.8125</v>
+      </c>
+      <c r="B18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
+        <v>45025.3125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
+        <v>45025.8125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2">
+        <v>45026.3125</v>
+      </c>
+      <c r="B21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2">
+        <v>45026.8125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
+        <v>45046.8125</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
+        <v>45047.3125</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2">
+        <v>45047.8125</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2">
+        <v>45088.8125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2">
+        <v>45089.3125</v>
+      </c>
+      <c r="B27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2">
+        <v>45089.8125</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2">
+        <v>45156.8125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2">
+        <v>45157.3125</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2">
+        <v>45157.8125</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2">
+        <v>45158.8125</v>
+      </c>
+      <c r="B32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2">
+        <v>45159.3125</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2">
+        <v>45159.8125</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
+        <v>45165.8125</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
+        <v>45166.3125</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
+        <v>45166.8125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2">
+        <v>45230.8125</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2">
+        <v>45231.3125</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
+        <v>45231.8125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
+        <v>45232.3125</v>
+      </c>
+      <c r="B41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <v>45232.8125</v>
+      </c>
+      <c r="B42" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2">
+        <v>45256.8125</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
+        <v>45257.3125</v>
+      </c>
+      <c r="B44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2">
+        <v>45257.8125</v>
+      </c>
+      <c r="B45" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2">
+        <v>45259.8125</v>
+      </c>
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2">
+        <v>45260.3125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
+        <v>45260.8125</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
+        <v>45267.8125</v>
+      </c>
+      <c r="B49" t="s">
+        <v>193</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2">
+        <v>45268.3125</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
+        <v>45268.8125</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2">
+        <v>45283.8125</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2">
+        <v>45284.3125</v>
+      </c>
+      <c r="B53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2">
+        <v>45284.8125</v>
+      </c>
+      <c r="B54" t="s">
+        <v>195</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2">
+        <v>45285.3125</v>
+      </c>
+      <c r="B55" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2">
+        <v>45285.8125</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2">
+        <v>45286.3125</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2">
+        <v>45286.8125</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2">
+        <v>45289.8125</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2">
+        <v>45290.3125</v>
+      </c>
+      <c r="B60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2">
+        <v>45290.8125</v>
+      </c>
+      <c r="B61" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
+        <v>45291.3125</v>
+      </c>
+      <c r="B62" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2">
+        <v>45291.8125</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2">
+        <v>45019.3125</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2">
+        <v>45020.3125</v>
+      </c>
+      <c r="B65" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2">
+        <v>45021.3125</v>
+      </c>
+      <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
+        <v>45027.3125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2">
+        <v>45028.3125</v>
+      </c>
+      <c r="B68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
+        <v>45029.3125</v>
+      </c>
+      <c r="B69" t="s">
+        <v>196</v>
+      </c>
+      <c r="C69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
+        <v>45029.8125</v>
+      </c>
+      <c r="B70" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
+        <v>45030.3125</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
+        <v>45030.8125</v>
+      </c>
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
+        <v>45033.3125</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2">
+        <v>45035.3125</v>
+      </c>
+      <c r="B74" t="s">
+        <v>198</v>
+      </c>
+      <c r="C74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2">
+        <v>45036.3125</v>
+      </c>
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2">
+        <v>45036.8125</v>
+      </c>
+      <c r="B76" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
+        <v>45042.3125</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
+        <v>45050.3125</v>
+      </c>
+      <c r="B78" t="s">
+        <v>126</v>
+      </c>
+      <c r="C78" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2">
+        <v>45053.8125</v>
+      </c>
+      <c r="B79" t="s">
+        <v>197</v>
+      </c>
+      <c r="C79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2">
+        <v>45055.3125</v>
+      </c>
+      <c r="B80" t="s">
+        <v>199</v>
+      </c>
+      <c r="C80" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2">
+        <v>45060.8125</v>
+      </c>
+      <c r="B81" t="s">
+        <v>68</v>
+      </c>
+      <c r="C81" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2">
+        <v>45064.3125</v>
+      </c>
+      <c r="B82" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
+        <v>45071.8125</v>
+      </c>
+      <c r="B83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
+        <v>45124.3125</v>
+      </c>
+      <c r="B84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2">
+        <v>45124.8125</v>
+      </c>
+      <c r="B85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>45125.3125</v>
+      </c>
+      <c r="B86" t="s">
+        <v>155</v>
+      </c>
+      <c r="C86" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
+        <v>45125.8125</v>
+      </c>
+      <c r="B87" t="s">
+        <v>199</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2">
+        <v>45126.3125</v>
+      </c>
+      <c r="B88" t="s">
+        <v>194</v>
+      </c>
+      <c r="C88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2">
+        <v>45126.8125</v>
+      </c>
+      <c r="B89" t="s">
+        <v>37</v>
+      </c>
+      <c r="C89" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2">
+        <v>45127.3125</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2">
+        <v>45127.8125</v>
+      </c>
+      <c r="B91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C91" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
+        <v>45128.3125</v>
+      </c>
+      <c r="B92" t="s">
+        <v>123</v>
+      </c>
+      <c r="C92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>45128.8125</v>
+      </c>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C109"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="19.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -5338,842 +6488,1908 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2">
-        <v>44927.3125</v>
+        <v>45292.3125</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2">
-        <v>44927.8125</v>
+        <v>45292.8125</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2">
-        <v>44928.3125</v>
+        <v>45331.8125</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2">
-        <v>44928.8125</v>
+        <v>45332.3125</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2">
-        <v>44981.8125</v>
+        <v>45332.8125</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>45378.8125</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>45379.3125</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>45379.8125</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>45380.3125</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>45380.8125</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>45381.3125</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>45381.8125</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="11">
+        <v>45355.3125</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="11">
+        <v>45357.3125</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="11">
+        <v>45358.3125</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11">
+        <v>45362.3125</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11">
+        <v>45363.3125</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11">
+        <v>45364.3125</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11">
+        <v>45365.3125</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11">
+        <v>45370.3125</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11">
+        <v>45371.3125</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11">
+        <v>45377.3125</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11">
+        <v>45378.3125</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="8">
+        <v>45383.3125</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="8">
+        <v>45384.3125</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="8">
+        <v>45385.3125</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="8">
+        <v>45386.3125</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="8">
+        <v>45390.3125</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="8">
+        <v>45393.3125</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="8">
+        <v>45394.3125</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="8">
+        <v>45395.3125</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="8">
+        <v>45397.3125</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="8">
+        <v>45398.3125</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="8">
+        <v>45399.3125</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8">
+        <v>45400.3125</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="8">
+        <v>45402.3125</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="8">
+        <v>45403.8125</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="8">
+        <v>45404.3125</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="8">
+        <v>45405.3125</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="8">
+        <v>45406.3125</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8">
+        <v>45407.3125</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="8">
+        <v>45408.3125</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
+        <v>45390.8125</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2">
+        <v>45391.3125</v>
+      </c>
+      <c r="B45" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2">
+        <v>45391.8125</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2">
+        <v>45412.8125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
+        <v>45413.3125</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
+        <v>45413.8125</v>
+      </c>
+      <c r="B49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="9">
+        <v>45418.3125</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="9">
+        <v>45419.3125</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="9">
+        <v>45420.3125</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="9">
+        <v>45421.3125</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="9">
+        <v>45423.8125</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="9">
+        <v>45426.3125</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="9">
+        <v>45427.3125</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="9">
+        <v>45428.3125</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="9">
+        <v>45431.8125</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="9">
+        <v>45433.3125</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="9">
+        <v>45434.3125</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="9">
+        <v>45435.3125</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="9">
+        <v>45438.8125</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="9">
+        <v>45439.3125</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="9">
+        <v>45440.3125</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="9">
+        <v>45449.3125</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="11">
+        <v>45454.3125</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
+        <v>45454.8125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2">
+        <v>45455.3125</v>
+      </c>
+      <c r="B68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
+        <v>45455.8125</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
+        <v>45522.8125</v>
+      </c>
+      <c r="B70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
+        <v>45523.3125</v>
+      </c>
+      <c r="B71" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
+        <v>45523.8125</v>
+      </c>
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
+        <v>45524.8125</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2">
+        <v>45525.3125</v>
+      </c>
+      <c r="B74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2">
+        <v>45525.8125</v>
+      </c>
+      <c r="B75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2">
+        <v>45529.8125</v>
+      </c>
+      <c r="B76" t="s">
+        <v>198</v>
+      </c>
+      <c r="C76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
+        <v>45530.3125</v>
+      </c>
+      <c r="B77" t="s">
+        <v>199</v>
+      </c>
+      <c r="C77" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
+        <v>45530.8125</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2">
+        <v>45542.3125</v>
+      </c>
+      <c r="B79" t="s">
+        <v>193</v>
+      </c>
+      <c r="C79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2">
+        <v>45596.8125</v>
+      </c>
+      <c r="B80" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2">
+        <v>45597.3125</v>
+      </c>
+      <c r="B81" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2">
+        <v>45597.8125</v>
+      </c>
+      <c r="B82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
+        <v>45598.3125</v>
+      </c>
+      <c r="B83" t="s">
+        <v>203</v>
+      </c>
+      <c r="C83" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
+        <v>45598.8125</v>
+      </c>
+      <c r="B84" t="s">
+        <v>194</v>
+      </c>
+      <c r="C84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2">
+        <v>45605.3125</v>
+      </c>
+      <c r="B85" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>45625.8125</v>
+      </c>
+      <c r="B86" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
+        <v>45626.3125</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2">
+        <v>45626.8125</v>
+      </c>
+      <c r="B88" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2">
+        <v>45633.3125</v>
+      </c>
+      <c r="B89" t="s">
+        <v>193</v>
+      </c>
+      <c r="C89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2">
+        <v>45633.8125</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2">
+        <v>45634.3125</v>
+      </c>
+      <c r="B91" t="s">
+        <v>208</v>
+      </c>
+      <c r="C91" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
+        <v>45634.8125</v>
+      </c>
+      <c r="B92" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>45649.8125</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2">
+        <v>45650.3125</v>
+      </c>
+      <c r="B94" t="s">
+        <v>209</v>
+      </c>
+      <c r="C94" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2">
+        <v>45650.8125</v>
+      </c>
+      <c r="B95" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2">
+        <v>45651.3125</v>
+      </c>
+      <c r="B96" t="s">
+        <v>131</v>
+      </c>
+      <c r="C96" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="2">
+        <v>45651.8125</v>
+      </c>
+      <c r="B97" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="2">
+        <v>45652.3125</v>
+      </c>
+      <c r="B98" t="s">
+        <v>68</v>
+      </c>
+      <c r="C98" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="2">
+        <v>45652.8125</v>
+      </c>
+      <c r="B99" t="s">
+        <v>28</v>
+      </c>
+      <c r="C99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="2">
+        <v>45653.3125</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2">
+        <v>45653.8125</v>
+      </c>
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="2">
+        <v>45654.3125</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2">
+        <v>45654.8125</v>
+      </c>
+      <c r="B103" t="s">
+        <v>87</v>
+      </c>
+      <c r="C103" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
+        <v>45655.3125</v>
+      </c>
+      <c r="B104" t="s">
+        <v>194</v>
+      </c>
+      <c r="C104" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2">
+        <v>45655.8125</v>
+      </c>
+      <c r="B105" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="2">
+        <v>45656.3125</v>
+      </c>
+      <c r="B106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
+        <v>45656.8125</v>
+      </c>
+      <c r="B107" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
+        <v>45657.3125</v>
+      </c>
+      <c r="B108" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2">
+        <v>45657.8125</v>
+      </c>
+      <c r="B109" t="s">
+        <v>193</v>
+      </c>
+      <c r="C109" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>45668.3125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>45719.3125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>45933.3125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>45738.3125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>45727.3125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2">
-        <v>44962.3125</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="3">
+        <v>45728.3125</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5">
+        <v>45729.3125</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>45735.3125</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5">
+        <v>45736.3125</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>45742.3125</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5">
+        <v>45756.3125</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="5">
+        <v>45764.3125</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="5">
+        <v>45765.3125</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2">
-        <v>44968.3125</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="5">
+        <v>45749.3125</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="5">
+        <v>45750.3125</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="5">
+        <v>45751.3125</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="5">
+        <v>45753.3125</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5">
+        <v>45755.3125</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5">
+        <v>45757.3125</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5">
+        <v>45763.3125</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="5">
+        <v>45771.3125</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5">
+        <v>45777.3125</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="5">
+        <v>45748.3125</v>
+      </c>
+      <c r="B24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" t="s">
         <v>193</v>
       </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2">
-        <v>44969.3125</v>
-      </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>44982.3125</v>
-      </c>
-      <c r="B10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>44982.8125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>193</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>45021.8125</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>45022.3125</v>
-      </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2">
-        <v>45022.8125</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2">
-        <v>45023.3125</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2">
-        <v>45023.8125</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2">
-        <v>45024.3125</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2">
-        <v>45024.8125</v>
-      </c>
-      <c r="B18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2">
-        <v>45025.3125</v>
-      </c>
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2">
-        <v>45025.8125</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2">
-        <v>45026.3125</v>
-      </c>
-      <c r="B21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2">
-        <v>45026.8125</v>
-      </c>
-      <c r="B22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2">
-        <v>45046.8125</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2">
-        <v>45047.3125</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="2">
-        <v>45047.8125</v>
+      <c r="A25" s="5">
+        <v>45784.3125</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2">
-        <v>45088.8125</v>
+      <c r="A26" s="5">
+        <v>45792.3125</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="2">
-        <v>45089.3125</v>
-      </c>
-      <c r="B27" t="s">
-        <v>194</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="2">
-        <v>45089.8125</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="2">
-        <v>45156.8125</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="2">
-        <v>45157.3125</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2">
-        <v>45157.8125</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>196</v>
-      </c>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5">
+        <v>45798.3125</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5">
+        <v>45804.3125</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5">
+        <v>45800.3125</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5">
+        <v>45825.3125</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5">
+        <v>45832.3125</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2">
-        <v>45158.8125</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>74</v>
+      <c r="A32" s="5">
+        <v>45810.3125</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2">
-        <v>45159.3125</v>
-      </c>
-      <c r="B33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
+      <c r="A33" s="5">
+        <v>45854.3125</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2">
-        <v>45159.8125</v>
-      </c>
-      <c r="B34" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" t="s">
-        <v>94</v>
+      <c r="A34" s="5">
+        <v>45860.3125</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2">
-        <v>45165.8125</v>
-      </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>87</v>
-      </c>
+      <c r="A35" s="5"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2">
-        <v>45166.3125</v>
-      </c>
-      <c r="B36" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" t="s">
-        <v>54</v>
-      </c>
+      <c r="A36" s="5"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2">
-        <v>45166.8125</v>
-      </c>
-      <c r="B37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" t="s">
-        <v>36</v>
-      </c>
+      <c r="A37" s="5"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2">
-        <v>45230.8125</v>
-      </c>
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2">
-        <v>45231.3125</v>
-      </c>
-      <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
-        <v>45</v>
-      </c>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2">
-        <v>45231.8125</v>
-      </c>
-      <c r="B40" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" t="s">
-        <v>28</v>
-      </c>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2">
-        <v>45232.3125</v>
-      </c>
-      <c r="B41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C41" t="s">
-        <v>64</v>
-      </c>
+      <c r="A41" s="8"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2">
-        <v>45232.8125</v>
-      </c>
-      <c r="B42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" t="s">
-        <v>131</v>
-      </c>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2">
-        <v>45256.8125</v>
-      </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" t="s">
-        <v>75</v>
-      </c>
+      <c r="A43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2">
-        <v>45257.3125</v>
-      </c>
-      <c r="B44" t="s">
-        <v>197</v>
-      </c>
-      <c r="C44" t="s">
-        <v>155</v>
-      </c>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2">
-        <v>45257.8125</v>
-      </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
+      <c r="A45" s="8"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2">
-        <v>45259.8125</v>
-      </c>
-      <c r="B46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s">
-        <v>194</v>
-      </c>
+      <c r="A46" s="8"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2">
-        <v>45260.3125</v>
-      </c>
-      <c r="B47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" t="s">
-        <v>123</v>
-      </c>
+      <c r="A47" s="8"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2">
-        <v>45260.8125</v>
-      </c>
-      <c r="B48" t="s">
-        <v>128</v>
-      </c>
-      <c r="C48" t="s">
-        <v>70</v>
-      </c>
+      <c r="A48" s="8"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2">
-        <v>45267.8125</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="2">
-        <v>45268.3125</v>
-      </c>
-      <c r="B50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="2">
-        <v>45268.8125</v>
-      </c>
-      <c r="B51" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="2">
-        <v>45283.8125</v>
-      </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="2">
-        <v>45284.3125</v>
-      </c>
-      <c r="B53" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="2">
-        <v>45284.8125</v>
-      </c>
-      <c r="B54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="2">
-        <v>45285.3125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" t="s">
-        <v>199</v>
-      </c>
+      <c r="A49" s="8"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2">
-        <v>45285.8125</v>
-      </c>
-      <c r="B56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" t="s">
-        <v>63</v>
-      </c>
+      <c r="A56" s="9"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2">
-        <v>45286.3125</v>
-      </c>
-      <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" t="s">
-        <v>199</v>
-      </c>
+      <c r="A57" s="9"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2">
-        <v>45286.8125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" t="s">
-        <v>91</v>
-      </c>
+      <c r="A58" s="9"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="2">
-        <v>45289.8125</v>
-      </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" t="s">
-        <v>106</v>
-      </c>
+      <c r="A59" s="9"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2">
-        <v>45290.3125</v>
-      </c>
-      <c r="B60" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" t="s">
-        <v>34</v>
-      </c>
+      <c r="A60" s="9"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2">
-        <v>45290.8125</v>
-      </c>
-      <c r="B61" t="s">
-        <v>76</v>
-      </c>
-      <c r="C61" t="s">
-        <v>155</v>
-      </c>
+      <c r="A61" s="9"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2">
-        <v>45291.3125</v>
-      </c>
-      <c r="B62" t="s">
-        <v>196</v>
-      </c>
-      <c r="C62" t="s">
-        <v>74</v>
-      </c>
+      <c r="A62" s="9"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="2">
-        <v>45291.8125</v>
-      </c>
-      <c r="B63" t="s">
-        <v>55</v>
-      </c>
-      <c r="C63" t="s">
-        <v>94</v>
-      </c>
+      <c r="A63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="3">
-        <v>45019.3125</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>195</v>
-      </c>
+      <c r="A64" s="9"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="3">
-        <v>45020.3125</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>196</v>
-      </c>
+      <c r="A65" s="9"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="3">
-        <v>45021.3125</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A66" s="9"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="3">
-        <v>45027.3125</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="A67" s="9"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="3">
-        <v>45028.3125</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A68" s="9"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="3">
-        <v>45029.3125</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="A69" s="9"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="3">
-        <v>45029.8125</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>96</v>
-      </c>
+      <c r="A70" s="9"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="3">
-        <v>45030.3125</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>198</v>
-      </c>
+      <c r="A71" s="9"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="3">
-        <v>45030.8125</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="3">
-        <v>45033.3125</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="3">
-        <v>45035.3125</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="3">
-        <v>45036.3125</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="3">
-        <v>45036.8125</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="3">
-        <v>45042.3125</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="A72" s="11"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="2"/>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="2"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="2"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>